<commit_message>
Contenido Teorico capa 2
</commit_message>
<xml_diff>
--- a/docs/OSI_01-capa_fisica.xlsx
+++ b/docs/OSI_01-capa_fisica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\redes\saves\ccna-s-15\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{076A3FD4-135F-4B8E-AF5F-3DC8769B5AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305E3730-33F2-4AF5-B999-009652941721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{9A62988E-56DA-4ABE-8EFC-23F0AD723830}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
   <si>
     <t>TIA-568A</t>
   </si>
@@ -269,6 +269,33 @@
   </si>
   <si>
     <t>FRECUENCIA DE DATOS</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada</t>
+  </si>
+  <si>
+    <t>El alto de la sinusoide aumenta y disminuye</t>
+  </si>
+  <si>
+    <t>Frecuencia modulada</t>
+  </si>
+  <si>
+    <t>El ancho de la sinusoide crece y decrece</t>
+  </si>
+  <si>
+    <t>Modulacion de Fase</t>
+  </si>
+  <si>
+    <t>Utiliza una señal como guia y otra para datos</t>
   </si>
 </sst>
 </file>
@@ -579,7 +606,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -681,6 +708,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -705,39 +759,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="14" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -752,6 +779,12 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1074,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7651BEDB-B928-44A9-A7A9-86D2E8AFC30B}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:K17"/>
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,35 +1135,35 @@
       <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="75"/>
-      <c r="I2" s="58" t="s">
+      <c r="F2" s="57"/>
+      <c r="I2" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="58" t="s">
+      <c r="K2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="66" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="57"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="75"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="58"/>
+      <c r="I3" s="67"/>
       <c r="J3" s="16"/>
-      <c r="K3" s="58"/>
-      <c r="M3" s="57"/>
+      <c r="K3" s="67"/>
+      <c r="M3" s="66"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -1154,15 +1187,15 @@
       <c r="G4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="72" t="s">
+      <c r="I4" s="65" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="15"/>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="61" t="s">
         <v>9</v>
       </c>
       <c r="L4" s="15"/>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="61" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1188,11 +1221,11 @@
       <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="68"/>
+      <c r="I5" s="61"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="68"/>
+      <c r="K5" s="61"/>
       <c r="L5" s="15"/>
-      <c r="M5" s="68"/>
+      <c r="M5" s="61"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1216,11 +1249,11 @@
       <c r="G6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="68"/>
+      <c r="I6" s="61"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="68"/>
+      <c r="K6" s="61"/>
       <c r="L6" s="15"/>
-      <c r="M6" s="68"/>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1244,11 +1277,11 @@
       <c r="G7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="68"/>
+      <c r="I7" s="61"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="68"/>
+      <c r="K7" s="61"/>
       <c r="L7" s="15"/>
-      <c r="M7" s="68"/>
+      <c r="M7" s="61"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -1272,11 +1305,11 @@
       <c r="G8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="68"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="68"/>
+      <c r="K8" s="61"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="68"/>
+      <c r="M8" s="61"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1300,11 +1333,11 @@
       <c r="G9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="68"/>
+      <c r="I9" s="61"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="68"/>
+      <c r="K9" s="61"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="68"/>
+      <c r="M9" s="61"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
@@ -1328,11 +1361,11 @@
       <c r="G10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="68"/>
+      <c r="I10" s="61"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="68"/>
+      <c r="K10" s="61"/>
       <c r="L10" s="15"/>
-      <c r="M10" s="68"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1356,102 +1389,105 @@
       <c r="G11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="68"/>
+      <c r="I11" s="61"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="68"/>
+      <c r="K11" s="61"/>
       <c r="L11" s="15"/>
-      <c r="M11" s="68"/>
+      <c r="M11" s="61"/>
     </row>
     <row r="12" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M12" s="68"/>
+      <c r="M12" s="61"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="62" t="s">
+      <c r="C13" s="60"/>
+      <c r="D13" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="M13" s="68"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="73"/>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="69"/>
-      <c r="D14" s="59" t="s">
+      <c r="C14" s="62"/>
+      <c r="D14" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
-      <c r="M14" s="68"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="70"/>
+      <c r="M14" s="61"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="65" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="66"/>
-      <c r="K15" s="66"/>
-      <c r="M15" s="68"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="M15" s="61"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="70" t="s">
+      <c r="B16" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71" t="s">
+      <c r="C16" s="63"/>
+      <c r="D16" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="M16" s="68"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="65" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="66"/>
-      <c r="K17" s="66"/>
-      <c r="M17" s="68"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="M17" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="D17:K17"/>
@@ -1468,9 +1504,6 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="D14:K14"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1480,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFDD7A3E-DEE6-4290-890F-1E9A92653B68}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O12" sqref="H12:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,6 +1795,19 @@
       <c r="G13" s="49" t="s">
         <v>73</v>
       </c>
+      <c r="I13" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="74" t="s">
+        <v>84</v>
+      </c>
+      <c r="K13" s="75"/>
+      <c r="L13" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="82"/>
+      <c r="N13" s="82"/>
+      <c r="O13" s="82"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B14" s="39" t="s">
@@ -1782,6 +1828,19 @@
       <c r="G14" s="50" t="s">
         <v>38</v>
       </c>
+      <c r="I14" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="J14" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14" s="75"/>
+      <c r="L14" s="82" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="40" t="s">
@@ -1802,9 +1861,25 @@
       <c r="G15" s="52" t="s">
         <v>44</v>
       </c>
+      <c r="I15" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="74" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="75"/>
+      <c r="L15" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B12:G12"/>

</xml_diff>